<commit_message>
adding data driven process executor
</commit_message>
<xml_diff>
--- a/DataDrivenPRocessExec.xlsx
+++ b/DataDrivenPRocessExec.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cocianm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\junit-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B56C531-2F12-4088-970A-087D9911F7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9B14D5-6BED-4C52-AB22-98B2895B3BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Executable</t>
   </si>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,6 +400,9 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -407,6 +410,9 @@
       </c>
       <c r="B3" t="s">
         <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>